<commit_message>
FlightEndDate validation and isfuture Date Validation code was done
</commit_message>
<xml_diff>
--- a/cypress/fixtures/rapp.xlsx
+++ b/cypress/fixtures/rapp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chandan.chamun\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sathishkumar.thiruma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD525E0-06DF-48F0-90BC-89A8AD5EC2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789A5618-3EEC-4D2A-8918-B7F280F98760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SocialDealerOrders" sheetId="2" r:id="rId1"/>
@@ -1740,88 +1740,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CO9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="35.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.77734375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="73.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="38.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="73.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="255.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.36328125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="36" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.6328125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="182.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="69.88671875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="122.109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="139.109375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="71.109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="182.90625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="69.90625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="122.08984375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="139.08984375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="71.08984375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.54296875" bestFit="1" customWidth="1"/>
     <col min="43" max="45" width="140" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="23" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="170.21875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="53" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="255.81640625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="170.1796875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="51" max="53" width="255.81640625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="23" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="170.21875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="59" max="61" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="255.81640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="170.1796875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="59" max="61" width="255.81640625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="23" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="170.21875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="67" max="69" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="255.81640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="170.1796875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="67" max="69" width="255.81640625" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="23" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="255.81640625" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="26" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="162.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="75" max="77" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="162.6328125" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="75" max="77" width="255.81640625" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="23" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="255.81640625" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="26" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="162.6640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="83" max="85" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="162.6328125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="83" max="85" width="255.81640625" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="23" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="255.81640625" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="26" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="162.6640625" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="91" max="93" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="162.6328125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="91" max="93" width="255.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>147</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="5" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>218</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>266</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="7" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>319</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="8" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>365</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:93" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:93" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>400</v>
       </c>

</xml_diff>